<commit_message>
aula 04 atualização pacotes
</commit_message>
<xml_diff>
--- a/data/dados_turmas.xlsx
+++ b/data/dados_turmas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="18">
   <si>
     <t>F</t>
   </si>
@@ -421,11 +421,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" sqref="A1:F1048576"/>
+      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +501,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>3</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>3</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>3</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>3</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>3</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>3</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>0</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>3</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>3</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>0</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>3</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>0</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>0</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>0</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>0</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>3</v>
@@ -961,7 +961,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>0</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>3</v>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>3</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>3</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>3</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>3</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>3</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>3</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>3</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>0</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>0</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>3</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>3</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>3</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>0</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>3</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>3</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>3</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>0</v>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>3</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>3</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>0</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>3</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>3</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>3</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>3</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>3</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>0</v>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>3</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>3</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>0</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>0</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>0</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>3</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>3</v>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>3</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>3</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>0</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>0</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>0</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>0</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>3</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>0</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>0</v>
@@ -1837,6 +1837,26 @@
       </c>
       <c r="F70" s="3">
         <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>70</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="3">
+        <v>1.64</v>
+      </c>
+      <c r="F71" s="3">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
banco de dados 2023
</commit_message>
<xml_diff>
--- a/data/dados_turmas.xlsx
+++ b/data/dados_turmas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="18">
   <si>
     <t>F</t>
   </si>
@@ -421,11 +421,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2019,6 +2019,26 @@
         <v>24</v>
       </c>
     </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="F80" s="3">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>